<commit_message>
Mac update 2.15 13.30
</commit_message>
<xml_diff>
--- a/ct/logs/segcapsr3/traincaps.xlsx
+++ b/ct/logs/segcapsr3/traincaps.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17540" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="26" sheetId="1" r:id="rId1"/>
@@ -739,11 +739,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-92690944"/>
-        <c:axId val="-92882000"/>
+        <c:axId val="-48961440"/>
+        <c:axId val="-120076400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-92690944"/>
+        <c:axId val="-48961440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -817,7 +817,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-92882000"/>
+        <c:crossAx val="-120076400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -826,7 +826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-92882000"/>
+        <c:axId val="-120076400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.25"/>
@@ -908,7 +908,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-92690944"/>
+        <c:crossAx val="-48961440"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1094,10 +1094,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'26'!$D$2:$D$40</c:f>
+              <c:f>'26'!$D$2:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.00807442054494501</c:v>
                 </c:pt>
@@ -1175,45 +1175,6 @@
                 </c:pt>
                 <c:pt idx="25" formatCode="General">
                   <c:v>0.908962060332298</c:v>
-                </c:pt>
-                <c:pt idx="26" formatCode="General">
-                  <c:v>0.918945491075515</c:v>
-                </c:pt>
-                <c:pt idx="27" formatCode="General">
-                  <c:v>0.924488268136978</c:v>
-                </c:pt>
-                <c:pt idx="28" formatCode="General">
-                  <c:v>0.926954695343971</c:v>
-                </c:pt>
-                <c:pt idx="29" formatCode="General">
-                  <c:v>0.929785791277885</c:v>
-                </c:pt>
-                <c:pt idx="30" formatCode="General">
-                  <c:v>0.928311052441597</c:v>
-                </c:pt>
-                <c:pt idx="31" formatCode="General">
-                  <c:v>0.928260118961334</c:v>
-                </c:pt>
-                <c:pt idx="32" formatCode="General">
-                  <c:v>0.92939108633995</c:v>
-                </c:pt>
-                <c:pt idx="33" formatCode="General">
-                  <c:v>0.930954586863517</c:v>
-                </c:pt>
-                <c:pt idx="34" formatCode="General">
-                  <c:v>0.930065424442291</c:v>
-                </c:pt>
-                <c:pt idx="35" formatCode="General">
-                  <c:v>0.926665329098701</c:v>
-                </c:pt>
-                <c:pt idx="36" formatCode="General">
-                  <c:v>0.929283975481987</c:v>
-                </c:pt>
-                <c:pt idx="37" formatCode="General">
-                  <c:v>0.928425056219101</c:v>
-                </c:pt>
-                <c:pt idx="38" formatCode="General">
-                  <c:v>0.930361023783683</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1248,10 +1209,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'26'!$H$2:$H$40</c:f>
+              <c:f>'26'!$H$2:$H$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>1.96240176886242E-10</c:v>
                 </c:pt>
@@ -1329,45 +1290,6 @@
                 </c:pt>
                 <c:pt idx="25" formatCode="General">
                   <c:v>0.879347296555837</c:v>
-                </c:pt>
-                <c:pt idx="26" formatCode="General">
-                  <c:v>0.934156201283137</c:v>
-                </c:pt>
-                <c:pt idx="27" formatCode="General">
-                  <c:v>0.935465514659881</c:v>
-                </c:pt>
-                <c:pt idx="28" formatCode="General">
-                  <c:v>0.93977795044581</c:v>
-                </c:pt>
-                <c:pt idx="29" formatCode="General">
-                  <c:v>0.940420673290888</c:v>
-                </c:pt>
-                <c:pt idx="30" formatCode="General">
-                  <c:v>0.93776961962382</c:v>
-                </c:pt>
-                <c:pt idx="31" formatCode="General">
-                  <c:v>0.936771035194397</c:v>
-                </c:pt>
-                <c:pt idx="32" formatCode="General">
-                  <c:v>0.941555043061574</c:v>
-                </c:pt>
-                <c:pt idx="33" formatCode="General">
-                  <c:v>0.93635872999827</c:v>
-                </c:pt>
-                <c:pt idx="34" formatCode="General">
-                  <c:v>0.93693387111028</c:v>
-                </c:pt>
-                <c:pt idx="35" formatCode="General">
-                  <c:v>0.936367034912109</c:v>
-                </c:pt>
-                <c:pt idx="36" formatCode="General">
-                  <c:v>0.935562193393707</c:v>
-                </c:pt>
-                <c:pt idx="37" formatCode="General">
-                  <c:v>0.935945429404576</c:v>
-                </c:pt>
-                <c:pt idx="38" formatCode="General">
-                  <c:v>0.940756827592849</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1383,11 +1305,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-95471280"/>
-        <c:axId val="-118565632"/>
+        <c:axId val="-6034448"/>
+        <c:axId val="-6031328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-95471280"/>
+        <c:axId val="-6034448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1494,7 +1416,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-118565632"/>
+        <c:crossAx val="-6031328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1504,10 +1426,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-118565632"/>
+        <c:axId val="-6031328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.5"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1619,7 +1541,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-95471280"/>
+        <c:crossAx val="-6034448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2825,16 +2747,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>889000</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2855,16 +2777,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3151,8 +3073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" activeCellId="1" sqref="D1:D40 H1:H40"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H40" sqref="H28:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>

</xml_diff>